<commit_message>
changed discount rates to 5.0%
</commit_message>
<xml_diff>
--- a/data/income_groups.xlsx
+++ b/data/income_groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Documents\Studium - UW\PUBPOL 594 A - Economic Approaches To Environmental Management\Project\tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB0320-0FEC-4AA8-9556-E1A91910CF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32464A8-65BC-4912-AB3C-E1680A215567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{DD775888-F91C-4112-8121-71A92DE74290}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DD775888-F91C-4112-8121-71A92DE74290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70D2DBF-580B-46D9-BE63-61DC94AB5FBA}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,7 +618,7 @@
         <v>13600</v>
       </c>
       <c r="I2" s="3">
-        <f t="shared" ref="I2:I7" si="0">F2+G2*(E2-H2)</f>
+        <f>F2+G2*(E2-H2)</f>
         <v>1388.68</v>
       </c>
       <c r="J2" s="1">
@@ -630,7 +630,7 @@
         <v>1388.68</v>
       </c>
       <c r="L2" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M2" s="1">
         <v>0.23300000000000001</v>
@@ -683,7 +683,7 @@
         <v>13600</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I2:I7" si="0">F3+G3*(E3-H3)</f>
         <v>4153</v>
       </c>
       <c r="J3" s="1">
@@ -695,7 +695,7 @@
         <v>4153</v>
       </c>
       <c r="L3" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M3" s="1">
         <v>0.224</v>
@@ -760,7 +760,7 @@
         <v>7500</v>
       </c>
       <c r="L4" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M4" s="1">
         <v>0.16500000000000001</v>
@@ -825,7 +825,7 @@
         <v>7500</v>
       </c>
       <c r="L5" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M5" s="1">
         <v>0.123</v>
@@ -890,7 +890,7 @@
         <v>7500</v>
       </c>
       <c r="L6" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M6" s="1">
         <v>0.2</v>
@@ -955,7 +955,7 @@
         <v>7500</v>
       </c>
       <c r="L7" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M7" s="1">
         <v>5.5E-2</v>

</xml_diff>

<commit_message>
included custom discount rates
</commit_message>
<xml_diff>
--- a/data/income_groups.xlsx
+++ b/data/income_groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Documents\Studium - UW\PUBPOL 594 A - Economic Approaches To Environmental Management\Project\tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32464A8-65BC-4912-AB3C-E1680A215567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472896E6-E794-4B80-A39D-A0E909346685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DD775888-F91C-4112-8121-71A92DE74290}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>discount rate</t>
   </si>
@@ -96,15 +96,6 @@
   </si>
   <si>
     <t>average vehicle age [years]</t>
-  </si>
-  <si>
-    <t>average annual mileage per person (WA) [mi]</t>
-  </si>
-  <si>
-    <t>average annual mileage per person (U.S.) [mi]</t>
-  </si>
-  <si>
-    <t>average annual mileage per vehicle (WA) [mi]</t>
   </si>
   <si>
     <t>average annual mileage per vehicle (U.S.) [mi]</t>
@@ -511,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70D2DBF-580B-46D9-BE63-61DC94AB5FBA}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,10 +518,10 @@
     <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.26953125" customWidth="1"/>
     <col min="13" max="15" width="13.08984375" customWidth="1"/>
-    <col min="16" max="19" width="14" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -580,24 +571,15 @@
         <v>20</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -642,22 +624,13 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="P2" s="6">
-        <v>5043</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>7490</v>
-      </c>
-      <c r="R2" s="6">
-        <v>12908.873572</v>
-      </c>
-      <c r="S2" s="6">
-        <v>13363.344440000001</v>
-      </c>
-      <c r="T2" s="5">
+        <v>13000</v>
+      </c>
+      <c r="Q2" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -683,7 +656,7 @@
         <v>13600</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I2:I7" si="0">F3+G3*(E3-H3)</f>
+        <f t="shared" ref="I3:I7" si="0">F3+G3*(E3-H3)</f>
         <v>4153</v>
       </c>
       <c r="J3" s="1">
@@ -707,22 +680,13 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="P3" s="6">
-        <v>8640</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>9896</v>
-      </c>
-      <c r="R3" s="6">
-        <v>11605.807788</v>
-      </c>
-      <c r="S3" s="6">
-        <v>14350.869022999999</v>
-      </c>
-      <c r="T3" s="5">
+        <v>13000</v>
+      </c>
+      <c r="Q3" s="5">
         <v>11.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -772,22 +736,13 @@
         <v>0.16700000000000001</v>
       </c>
       <c r="P4" s="6">
-        <v>10107</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>10497</v>
-      </c>
-      <c r="R4" s="6">
-        <v>12433.704757</v>
-      </c>
-      <c r="S4" s="6">
-        <v>13821.181558</v>
-      </c>
-      <c r="T4" s="5">
+        <v>13000</v>
+      </c>
+      <c r="Q4" s="5">
         <v>10.7</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -837,22 +792,13 @@
         <v>0.154</v>
       </c>
       <c r="P5" s="6">
-        <v>9833</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>9920</v>
-      </c>
-      <c r="R5" s="6">
-        <v>11632.925692000001</v>
-      </c>
-      <c r="S5" s="6">
-        <v>12954.195089999999</v>
-      </c>
-      <c r="T5" s="5">
+        <v>13000</v>
+      </c>
+      <c r="Q5" s="5">
         <v>9.9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -902,27 +848,18 @@
         <v>0.34100000000000003</v>
       </c>
       <c r="P6" s="6">
-        <v>9040</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>9349</v>
-      </c>
-      <c r="R6" s="6">
-        <v>10959.760188</v>
-      </c>
-      <c r="S6" s="6">
-        <v>12622.201553999999</v>
-      </c>
-      <c r="T6" s="5">
+        <v>13000</v>
+      </c>
+      <c r="Q6" s="5">
         <v>8.9</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <v>200000</v>
@@ -967,18 +904,9 @@
         <v>0.13</v>
       </c>
       <c r="P7" s="6">
-        <v>8184</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>8097</v>
-      </c>
-      <c r="R7" s="6">
-        <v>10929.918250999999</v>
-      </c>
-      <c r="S7" s="6">
-        <v>11533.463019999999</v>
-      </c>
-      <c r="T7" s="5">
+        <v>13000</v>
+      </c>
+      <c r="Q7" s="5">
         <v>8.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added custom discount rate functionality to summary results tab
</commit_message>
<xml_diff>
--- a/data/income_groups.xlsx
+++ b/data/income_groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Documents\Studium - UW\PUBPOL 594 A - Economic Approaches To Environmental Management\Project\tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EA690C-32D6-4CC1-A2E6-2B3843168C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF5FEB6-F6E8-48CB-A670-E75BA913ADC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DD775888-F91C-4112-8121-71A92DE74290}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{DD775888-F91C-4112-8121-71A92DE74290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>